<commit_message>
Update Tekken 8 Moveset Editing Data.xlsx
</commit_message>
<xml_diff>
--- a/Tekken 8 Moveset Editing Data.xlsx
+++ b/Tekken 8 Moveset Editing Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cs\Documents\GitHub\Tekken8Movesets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D8FCDDC-DF47-4404-AF29-B7A2029B8E92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF69DCCC-EDF1-4DAD-82CD-CE5ABA0D4A7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6313,6 +6313,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -6320,9 +6323,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -13126,15 +13126,15 @@
   <dimension ref="A1:C147"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:C2"/>
+      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A59" sqref="A59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="30.7109375" customWidth="1"/>
     <col min="2" max="2" width="33.42578125" customWidth="1"/>
-    <col min="3" max="3" width="84.140625" customWidth="1"/>
+    <col min="3" max="3" width="91.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -13149,7 +13149,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="86" t="s">
+      <c r="A2" s="83" t="s">
         <v>924</v>
       </c>
       <c r="B2" s="82"/>
@@ -13709,7 +13709,7 @@
         <v>937</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="48">
         <v>2304</v>
       </c>
@@ -16010,7 +16010,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A2" s="83" t="s">
+      <c r="A2" s="84" t="s">
         <v>1090</v>
       </c>
       <c r="B2" s="82"/>
@@ -17076,7 +17076,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="84" t="s">
+      <c r="A2" s="85" t="s">
         <v>1162</v>
       </c>
       <c r="B2" s="82"/>
@@ -17162,25 +17162,25 @@
       </c>
     </row>
     <row r="13" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="84" t="s">
+      <c r="A13" s="85" t="s">
         <v>1174</v>
       </c>
       <c r="B13" s="82"/>
     </row>
     <row r="14" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A14" s="85" t="s">
+      <c r="A14" s="86" t="s">
         <v>1175</v>
       </c>
       <c r="B14" s="82"/>
     </row>
     <row r="15" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="84" t="s">
+      <c r="A15" s="85" t="s">
         <v>1176</v>
       </c>
       <c r="B15" s="82"/>
     </row>
     <row r="16" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A16" s="85" t="s">
+      <c r="A16" s="86" t="s">
         <v>1177</v>
       </c>
       <c r="B16" s="82"/>
@@ -17266,13 +17266,13 @@
       </c>
     </row>
     <row r="27" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="84" t="s">
+      <c r="A27" s="85" t="s">
         <v>1197</v>
       </c>
       <c r="B27" s="82"/>
     </row>
     <row r="28" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A28" s="85" t="s">
+      <c r="A28" s="86" t="s">
         <v>1198</v>
       </c>
       <c r="B28" s="82"/>
@@ -17310,7 +17310,7 @@
       </c>
     </row>
     <row r="33" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="84" t="s">
+      <c r="A33" s="85" t="s">
         <v>1207</v>
       </c>
       <c r="B33" s="82"/>
@@ -17468,7 +17468,7 @@
       </c>
     </row>
     <row r="53" spans="1:2" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A53" s="84" t="s">
+      <c r="A53" s="85" t="s">
         <v>1239</v>
       </c>
       <c r="B53" s="82"/>
@@ -17602,7 +17602,7 @@
       </c>
     </row>
     <row r="70" spans="1:2" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A70" s="84" t="s">
+      <c r="A70" s="85" t="s">
         <v>1263</v>
       </c>
       <c r="B70" s="82"/>
@@ -17648,7 +17648,7 @@
       </c>
     </row>
     <row r="76" spans="1:2" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A76" s="84" t="s">
+      <c r="A76" s="85" t="s">
         <v>1269</v>
       </c>
       <c r="B76" s="82"/>

</xml_diff>